<commit_message>
v0.63 spawn command added
</commit_message>
<xml_diff>
--- a/time plan.xlsx
+++ b/time plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4E2888-C2C8-4DB1-9F91-9DD67A43E195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5EAC43-24B7-45EA-B2A7-8CFD7294A3A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,7 +803,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.72 more updates. turn functionality nearly finished (moves broken)
</commit_message>
<xml_diff>
--- a/time plan.xlsx
+++ b/time plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5EAC43-24B7-45EA-B2A7-8CFD7294A3A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F01560-6D43-421C-AB85-5E354A4F58FC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -512,6 +512,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent1" xfId="7" builtinId="31"/>
@@ -803,7 +804,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1291,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="4"/>
+      <c r="K15" s="1"/>
       <c r="L15" s="4"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1316,7 +1317,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="4"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1343,8 +1344,8 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="4"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1531,10 +1532,10 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1557,8 +1558,8 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>

</xml_diff>